<commit_message>
working on weather data table
</commit_message>
<xml_diff>
--- a/figure/FS.Latitude.Table.xlsx
+++ b/figure/FS.Latitude.Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="8820" windowHeight="13540" tabRatio="500"/>
+    <workbookView xWindow="6660" yWindow="0" windowWidth="16580" windowHeight="12480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Station</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Oslo, NO</t>
+  </si>
+  <si>
+    <t>Jena, GM</t>
+  </si>
+  <si>
+    <t>Flyvestation, DA</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -524,86 +530,120 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="C6">
-        <v>52.47</v>
+        <v>50.926699999999997</v>
       </c>
       <c r="D6">
-        <v>9.68</v>
+        <v>11.584199999999999</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C7">
-        <v>53.046399999999998</v>
+        <v>52.47</v>
       </c>
       <c r="D7">
-        <v>8.7992000000000008</v>
+        <v>9.68</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>53.634999999999998</v>
+        <v>53.046399999999998</v>
       </c>
       <c r="D8">
-        <v>9.99</v>
+        <v>8.7992000000000008</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>43</v>
-      </c>
       <c r="C9">
-        <v>54.5289</v>
+        <v>53.634999999999998</v>
       </c>
       <c r="D9">
-        <v>9.5492000000000008</v>
+        <v>9.99</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <v>54.5289</v>
+      </c>
+      <c r="D10">
+        <v>9.5492000000000008</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>57.093000000000004</v>
+      </c>
+      <c r="D11">
+        <v>9.8490000000000002</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>94</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>59.942799999999998</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>10.720599999999999</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finalized weather data and uploaded figures to sweave file
</commit_message>
<xml_diff>
--- a/figure/FS.Latitude.Table.xlsx
+++ b/figure/FS.Latitude.Table.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26680" yWindow="4880" windowWidth="16580" windowHeight="12480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="31700" yWindow="2780" windowWidth="18340" windowHeight="14440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>Station</t>
   </si>
@@ -76,6 +78,30 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Anthony, KS</t>
+  </si>
+  <si>
+    <t>West Point, NE</t>
+  </si>
+  <si>
+    <t>Brookings, SD</t>
+  </si>
+  <si>
+    <t>Aberdeen, SD</t>
+  </si>
+  <si>
+    <t>Pembina</t>
+  </si>
+  <si>
+    <t>Hastings, NE</t>
+  </si>
+  <si>
+    <t>Yankton, SD</t>
+  </si>
+  <si>
+    <t>Grand Forks, ND</t>
   </si>
 </sst>
 </file>
@@ -454,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:E11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -656,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1030,4 +1056,478 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>414.5</v>
+      </c>
+      <c r="C2">
+        <v>37.155000000000001</v>
+      </c>
+      <c r="D2">
+        <v>-98.028199999999998</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>586.70000000000005</v>
+      </c>
+      <c r="C3">
+        <v>40.583329999999997</v>
+      </c>
+      <c r="D3">
+        <v>-98.35</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>399.3</v>
+      </c>
+      <c r="C4">
+        <v>41.844999999999999</v>
+      </c>
+      <c r="D4">
+        <v>-96.714100000000002</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>359.7</v>
+      </c>
+      <c r="C5">
+        <v>42.883330000000001</v>
+      </c>
+      <c r="D5">
+        <v>-97.35</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>497.4</v>
+      </c>
+      <c r="C6">
+        <v>44.325200000000002</v>
+      </c>
+      <c r="D6">
+        <v>-96.768600000000006</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>395.3</v>
+      </c>
+      <c r="C7">
+        <v>45.443300000000001</v>
+      </c>
+      <c r="D7">
+        <v>-98.412999999999997</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>253</v>
+      </c>
+      <c r="C8">
+        <v>47.933300000000003</v>
+      </c>
+      <c r="D8">
+        <v>-97.083330000000004</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>240.8</v>
+      </c>
+      <c r="C9">
+        <v>48.9711</v>
+      </c>
+      <c r="D9">
+        <v>-97.241600000000005</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>414.5</v>
+      </c>
+      <c r="C2">
+        <v>37.155000000000001</v>
+      </c>
+      <c r="D2">
+        <v>-98.028199999999998</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="1">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="1">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="1">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="1">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="1">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="1">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="1">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="1">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="1">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="1">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>586.70000000000005</v>
+      </c>
+      <c r="C15">
+        <v>40.583329999999997</v>
+      </c>
+      <c r="D15">
+        <v>-98.35</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="1">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="1">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="1">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="1">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="1">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>399.3</v>
+      </c>
+      <c r="C22">
+        <v>41.844999999999999</v>
+      </c>
+      <c r="D22">
+        <v>-96.714100000000002</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="1">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="1">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="1">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>359.7</v>
+      </c>
+      <c r="C27">
+        <v>42.883330000000001</v>
+      </c>
+      <c r="D27">
+        <v>-97.35</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="1">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="1">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="1">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>497.4</v>
+      </c>
+      <c r="C32">
+        <v>44.325200000000002</v>
+      </c>
+      <c r="D32">
+        <v>-96.768600000000006</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>395.3</v>
+      </c>
+      <c r="C33">
+        <v>45.443300000000001</v>
+      </c>
+      <c r="D33">
+        <v>-98.412999999999997</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E34" s="1">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35">
+        <v>253</v>
+      </c>
+      <c r="C35">
+        <v>47.933300000000003</v>
+      </c>
+      <c r="D35">
+        <v>-97.083330000000004</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>240.8</v>
+      </c>
+      <c r="C36">
+        <v>48.9711</v>
+      </c>
+      <c r="D36">
+        <v>-97.241600000000005</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made new lm for freq of false spring events
</commit_message>
<xml_diff>
--- a/figure/FS.Latitude.Table.xlsx
+++ b/figure/FS.Latitude.Table.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/springfreeze/figure/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31700" yWindow="2780" windowWidth="18340" windowHeight="14440" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +14,18 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="24">
   <si>
     <t>Station</t>
   </si>
@@ -108,10 +103,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,8 +145,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -143,7 +164,17 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,9 +515,9 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -520,7 +551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -537,7 +568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -554,7 +585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -571,7 +602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -588,7 +619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -605,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -622,7 +653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -639,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -656,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -675,6 +706,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -686,12 +722,12 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -725,42 +761,42 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="E3" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="E4" s="1">
         <v>1998</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="E5" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="E6" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="E7" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="E8" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="E9" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -777,42 +813,42 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="E11" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="E12" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="E13" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="E14" s="1">
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="E15" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="E16" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="E17" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -829,37 +865,37 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="E19" s="1">
         <v>1998</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="E20" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="E21" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -876,22 +912,22 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -908,32 +944,32 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="E33" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="E34" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -950,27 +986,27 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="E36" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="E37" s="1">
         <v>2005</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="E38" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="E39" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -987,22 +1023,22 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="E41" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="E42" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="E43" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +1055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -1036,7 +1072,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1055,6 +1091,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1066,9 +1107,9 @@
       <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1102,7 +1143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1119,7 +1160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1136,7 +1177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1153,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1170,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1187,7 +1228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1204,7 +1245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1223,6 +1264,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1231,15 +1277,15 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1273,67 +1319,103 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
       <c r="E3" s="1">
         <v>1990</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
       <c r="E4" s="1">
         <v>1994</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="1">
         <v>1995</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
       <c r="E6" s="1">
         <v>1996</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
       <c r="E8" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
       <c r="E9" s="1">
         <v>2003</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
       <c r="E10" s="1">
         <v>2006</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
       <c r="E11" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
       <c r="E12" s="1">
         <v>2009</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
       <c r="E13" s="1">
         <v>2013</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
       <c r="E14" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1350,37 +1432,55 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
       <c r="E16" s="1">
         <v>1999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
       <c r="E17" s="1">
         <v>2000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
       <c r="E18" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
       <c r="E19" s="1">
         <v>2005</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
       <c r="E20" s="1">
         <v>2006</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
       <c r="E21" s="1">
         <v>2009</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1397,27 +1497,39 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
       <c r="E23" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
       <c r="E24" s="1">
         <v>2005</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
       <c r="E25" s="1">
         <v>2006</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
       <c r="E26" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1434,27 +1546,39 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
       <c r="E28" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
       <c r="E29" s="1">
         <v>2004</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
       <c r="E30" s="1">
         <v>2005</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
       <c r="E31" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1471,7 +1595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1488,12 +1612,15 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
       <c r="E34" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1510,7 +1637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1529,5 +1656,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on latitudinal gradient
</commit_message>
<xml_diff>
--- a/figure/FS.Latitude.Table.xlsx
+++ b/figure/FS.Latitude.Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="12140" yWindow="0" windowWidth="25360" windowHeight="14000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="25">
   <si>
     <t>Station</t>
   </si>
@@ -97,13 +97,16 @@
   </si>
   <si>
     <t>Grand Forks, ND</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,6 +126,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,11 +168,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -509,15 +520,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,8 +544,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -550,8 +564,11 @@
       <c r="E2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -567,8 +584,11 @@
       <c r="E3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -584,8 +604,11 @@
       <c r="E4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -601,8 +624,11 @@
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -618,8 +644,11 @@
       <c r="E6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -635,8 +664,11 @@
       <c r="E7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -652,8 +684,11 @@
       <c r="E8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -669,25 +704,31 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>3</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>57.093000000000004</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>9.8490000000000002</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -701,6 +742,9 @@
         <v>10.720599999999999</v>
       </c>
       <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>0</v>
       </c>
     </row>
@@ -718,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1101,15 +1145,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1125,8 +1169,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1142,8 +1189,11 @@
       <c r="E2">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1159,8 +1209,11 @@
       <c r="E3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1176,8 +1229,11 @@
       <c r="E4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1193,8 +1249,11 @@
       <c r="E5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1210,8 +1269,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1227,8 +1289,11 @@
       <c r="E7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1244,8 +1309,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1260,6 +1328,9 @@
       </c>
       <c r="E9">
         <v>1</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +1347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
working on anovas and latitudinal gradient stuff
</commit_message>
<xml_diff>
--- a/figure/FS.Latitude.Table.xlsx
+++ b/figure/FS.Latitude.Table.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28016"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/springfreeze/figure/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12140" yWindow="0" windowWidth="25360" windowHeight="14000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="26000" yWindow="460" windowWidth="25360" windowHeight="14000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,18 +19,18 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="28">
   <si>
     <t>Station</t>
   </si>
@@ -100,6 +105,15 @@
   </si>
   <si>
     <t>new</t>
+  </si>
+  <si>
+    <t>250/60</t>
+  </si>
+  <si>
+    <t>50/250/60</t>
+  </si>
+  <si>
+    <t>50/250/75</t>
   </si>
 </sst>
 </file>
@@ -520,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,11 +558,29 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="F1">
+        <v>200</v>
+      </c>
+      <c r="G1">
+        <v>115</v>
+      </c>
+      <c r="H1">
+        <v>300</v>
+      </c>
+      <c r="I1">
+        <v>250</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -567,8 +599,26 @@
       <c r="F2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>16</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -587,8 +637,26 @@
       <c r="F3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -607,8 +675,26 @@
       <c r="F4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>13</v>
+      </c>
+      <c r="K4">
+        <v>22</v>
+      </c>
+      <c r="L4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -627,8 +713,26 @@
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -647,8 +751,26 @@
       <c r="F6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -667,8 +789,26 @@
       <c r="F7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -687,8 +827,26 @@
       <c r="F8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -707,8 +865,26 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="2" customFormat="1">
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -727,8 +903,26 @@
       <c r="F10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -747,14 +941,27 @@
       <c r="F11">
         <v>0</v>
       </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -766,12 +973,12 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -788,7 +995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -805,42 +1012,42 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E3" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="1">
         <v>1998</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E6" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E7" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E8" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E9" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -857,42 +1064,42 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E12" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E13" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E14" s="1">
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E15" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E16" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E17" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -909,37 +1116,37 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E19" s="1">
         <v>1998</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E20" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E21" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E22" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E23" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E24" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -956,22 +1163,22 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E26" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E27" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E28" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -988,32 +1195,32 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E30" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E31" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E32" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E33" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E34" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1030,27 +1237,27 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E36" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E37" s="1">
         <v>2005</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E38" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E39" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1067,22 +1274,22 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E41" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E42" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E43" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -1116,7 +1323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1135,11 +1342,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1147,13 +1349,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1173,7 +1375,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1193,7 +1395,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1213,7 +1415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1233,7 +1435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1253,7 +1455,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1273,7 +1475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1293,7 +1495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1313,7 +1515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1335,11 +1537,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1351,12 +1548,12 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1390,7 +1587,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1398,7 +1595,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1406,7 +1603,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1414,7 +1611,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1422,7 +1619,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1430,7 +1627,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1438,7 +1635,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1446,7 +1643,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1454,7 +1651,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1462,7 +1659,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1470,7 +1667,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1478,7 +1675,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1486,7 +1683,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1503,7 +1700,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1511,7 +1708,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1519,7 +1716,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1527,7 +1724,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1535,7 +1732,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1543,7 +1740,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1551,7 +1748,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1568,7 +1765,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1576,7 +1773,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1584,7 +1781,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1592,7 +1789,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1600,7 +1797,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1617,7 +1814,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1625,7 +1822,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1633,7 +1830,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1641,7 +1838,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1649,7 +1846,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1666,7 +1863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1683,7 +1880,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -1691,7 +1888,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1708,7 +1905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1728,10 +1925,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on latitudinal gradient maps
</commit_message>
<xml_diff>
--- a/figure/FS.Latitude.Table.xlsx
+++ b/figure/FS.Latitude.Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26000" yWindow="460" windowWidth="25360" windowHeight="14000" tabRatio="500"/>
+    <workbookView xWindow="18780" yWindow="3380" windowWidth="25360" windowHeight="14000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="29">
   <si>
     <t>Station</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>50/250/75</t>
+  </si>
+  <si>
+    <t>fifty</t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -1347,15 +1350,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1374,8 +1377,11 @@
       <c r="F1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1394,8 +1400,11 @@
       <c r="F2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1414,8 +1423,11 @@
       <c r="F3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1434,8 +1446,11 @@
       <c r="F4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1454,8 +1469,11 @@
       <c r="F5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1474,8 +1492,11 @@
       <c r="F6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1494,8 +1515,11 @@
       <c r="F7">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1514,8 +1538,11 @@
       <c r="F8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1533,6 +1560,9 @@
       </c>
       <c r="F9">
         <v>11</v>
+      </c>
+      <c r="G9">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of work on latitudinal gradient
</commit_message>
<xml_diff>
--- a/figure/FS.Latitude.Table.xlsx
+++ b/figure/FS.Latitude.Table.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/springfreeze/figure/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="3380" windowWidth="25360" windowHeight="14000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="580" yWindow="0" windowWidth="25120" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="europe.lat.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
   <si>
     <t>Station</t>
   </si>
@@ -117,6 +112,15 @@
   </si>
   <si>
     <t>fifty</t>
+  </si>
+  <si>
+    <t>50/150/60</t>
+  </si>
+  <si>
+    <t>10/150-60</t>
+  </si>
+  <si>
+    <t>hf.gdd</t>
   </si>
 </sst>
 </file>
@@ -537,15 +541,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,8 +589,17 @@
       <c r="L1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -620,8 +636,17 @@
       <c r="L2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>33</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -658,8 +683,17 @@
       <c r="L3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>24</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -696,8 +730,17 @@
       <c r="L4">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <v>11</v>
+      </c>
+      <c r="O4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -734,8 +777,17 @@
       <c r="L5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>14</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -772,8 +824,17 @@
       <c r="L6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>21</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -810,8 +871,17 @@
       <c r="L7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>17</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -848,8 +918,17 @@
       <c r="L8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>16</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -886,8 +965,17 @@
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="2" customFormat="1">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -924,8 +1012,14 @@
       <c r="L10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -962,9 +1056,23 @@
       <c r="L11">
         <v>0</v>
       </c>
+      <c r="M11">
+        <v>7</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -976,12 +1084,12 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1015,42 +1123,42 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="E3" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="E4" s="1">
         <v>1998</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="E5" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="E6" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="E7" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="E8" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="E9" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1067,42 +1175,42 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="E11" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="E12" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="E13" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="E14" s="1">
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="E15" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="E16" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="E17" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1119,37 +1227,37 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="E19" s="1">
         <v>1998</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="E20" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="E21" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1166,22 +1274,22 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <v>2002</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1198,32 +1306,32 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <v>1997</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <v>2007</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="E33" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="E34" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1240,27 +1348,27 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="E36" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="E37" s="1">
         <v>2005</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="E38" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="E39" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1277,22 +1385,22 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="E41" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="E42" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="E43" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1309,7 +1417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -1326,7 +1434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1345,20 +1453,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1380,8 +1496,11 @@
       <c r="G1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1403,8 +1522,17 @@
       <c r="G2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1426,8 +1554,14 @@
       <c r="G3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1449,8 +1583,17 @@
       <c r="G4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1472,8 +1615,11 @@
       <c r="G5">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1495,8 +1641,17 @@
       <c r="G6">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1518,8 +1673,17 @@
       <c r="G7">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1541,8 +1705,11 @@
       <c r="G8">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1564,9 +1731,20 @@
       <c r="G9">
         <v>16</v>
       </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1578,12 +1756,12 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1600,7 +1778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1617,7 +1795,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1625,7 +1803,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1633,7 +1811,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1641,7 +1819,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1649,7 +1827,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1657,7 +1835,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1665,7 +1843,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1673,7 +1851,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1681,7 +1859,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1689,7 +1867,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1697,7 +1875,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1705,7 +1883,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1713,7 +1891,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1730,7 +1908,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1738,7 +1916,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1746,7 +1924,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1754,7 +1932,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1762,7 +1940,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1770,7 +1948,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1778,7 +1956,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1795,7 +1973,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1803,7 +1981,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1811,7 +1989,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1819,7 +1997,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1827,7 +2005,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1844,7 +2022,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1852,7 +2030,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1860,7 +2038,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1868,7 +2046,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1876,7 +2054,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1893,7 +2071,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1910,7 +2088,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -1918,7 +2096,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1935,7 +2113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1955,5 +2133,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>